<commit_message>
art of bop drumming
</commit_message>
<xml_diff>
--- a/assets uarm/chronomathesis2019b.xlsx
+++ b/assets uarm/chronomathesis2019b.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="12720" windowHeight="5895"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="12720" windowHeight="5895" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="agend" sheetId="1" r:id="rId1"/>
+    <sheet name="dias" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Semana</t>
   </si>
@@ -145,9 +145,6 @@
     <t>libro1y2</t>
   </si>
   <si>
-    <t>diogenes, helenismo</t>
-  </si>
-  <si>
     <t>laplace y leibniz</t>
   </si>
   <si>
@@ -188,6 +185,42 @@
   </si>
   <si>
     <t>mcIntyre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diogenes, helenismo, </t>
+  </si>
+  <si>
+    <t>teogonía, homero/McIntyre?</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>sábado</t>
+  </si>
+  <si>
+    <t>P. I. H.</t>
+  </si>
+  <si>
+    <t>7:20 - 9:00</t>
+  </si>
+  <si>
+    <t>13:00 - 14:20</t>
+  </si>
+  <si>
+    <t>PENS C</t>
   </si>
 </sst>
 </file>
@@ -579,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -635,12 +668,14 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" t="s">
@@ -664,7 +699,7 @@
         <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>16</v>
@@ -720,13 +755,13 @@
         <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
@@ -780,7 +815,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>28</v>
@@ -800,17 +835,17 @@
         <v>27</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -851,13 +886,13 @@
         <v>35</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" t="s">
@@ -881,7 +916,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>13</v>
@@ -908,7 +943,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>19</v>
@@ -985,7 +1020,7 @@
         <v>38</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>13</v>
@@ -1012,14 +1047,14 @@
         <v>38</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1044,7 +1079,7 @@
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1118,12 +1153,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>